<commit_message>
Correct typos & update offloading fig
</commit_message>
<xml_diff>
--- a/media/class_model_dict.xlsx
+++ b/media/class_model_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Manual\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA8FCA8-C4E5-40F7-A5D1-37093B5A0240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB91998E-B832-4B2F-9E3D-9A9918735552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Attributes</t>
+    <t>Attribute</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>